<commit_message>
sb sample name change
</commit_message>
<xml_diff>
--- a/data/soyabean/soya_part_1_2011_2012.xls.xlsx
+++ b/data/soyabean/soya_part_1_2011_2012.xls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coetzeeLA\OneDrive - University of the Free State\Documents\1. Research\Publications\Rothmann_LA\Sclerotinia silos\sagl_data\soyabean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufsacza-my.sharepoint.com/personal/coetzeela_ufs_ac_za/Documents/Documents/GitHub/sclerotia_silo/data/soyabean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{871EB333-39C1-4845-9A56-B5B3FEC70899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{871EB333-39C1-4845-9A56-B5B3FEC70899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55AFD7D8-21E7-418B-BB2B-C30DC5A11C91}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2850" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="23880" yWindow="-1680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="soya_part_1_2011_2012" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>Region</t>
   </si>
@@ -374,11 +374,14 @@
   <si>
     <t>T2 [max. value]</t>
   </si>
+  <si>
+    <t>No. of samples_scl</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -916,7 +919,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -938,9 +941,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1297,10 +1297,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1587,7 +1589,7 @@
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -1640,16 +1642,22 @@
       <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9">
+      <c r="B20" s="8">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8">
         <v>1</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9">
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
         <v>1</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9">
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1674,16 +1682,22 @@
       <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9">
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
         <v>1</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9">
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
         <v>1</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9">
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1708,16 +1722,22 @@
       <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9">
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
         <v>1</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
         <v>1</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9">
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1742,16 +1762,22 @@
       <c r="A26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9">
+      <c r="B26" s="8">
+        <v>0</v>
+      </c>
+      <c r="C26" s="8">
         <v>1</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9">
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
         <v>1</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9">
+      <c r="F26" s="8">
+        <v>0</v>
+      </c>
+      <c r="G26" s="8">
         <v>2</v>
       </c>
     </row>

</xml_diff>